<commit_message>
Worked on DT(Boost Converter, Current Sensor)
</commit_message>
<xml_diff>
--- a/HW-Module/Messergebnisse/ACS712-STROM-SPANNUNG.xlsx
+++ b/HW-Module/Messergebnisse/ACS712-STROM-SPANNUNG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Diplomarbeit\FaRiSmarthome\HW-Module\Messergebnisse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FaRiSmarthome\HW-Module\Messergebnisse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F18F85C-0307-49F6-8084-B31D697BBAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FD6AB7-85B7-4AB8-863A-7072B192525C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E26B9463-BDE3-4E68-BA94-F255C8AB7DFF}"/>
+    <workbookView xWindow="34669" yWindow="-3369" windowWidth="26300" windowHeight="15935" xr2:uid="{E26B9463-BDE3-4E68-BA94-F255C8AB7DFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>A</t>
   </si>
@@ -55,6 +55,12 @@
   <si>
     <t>Strom</t>
   </si>
+  <si>
+    <t>Gemessen</t>
+  </si>
+  <si>
+    <t>Von Excel generiert</t>
+  </si>
 </sst>
 </file>
 
@@ -72,12 +78,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,10 +110,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -148,7 +169,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>ACS712 - Hall</a:t>
+              <a:t>ACS712(20A) - Hall</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" baseline="0"/>
@@ -222,84 +243,144 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$A$2:$A$12</c:f>
+              <c:f>Tabelle1!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>-1</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>-2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>-3</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
                   <c:v>-4</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
                   <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$12</c:f>
+              <c:f>Tabelle1!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>2.6866666666666701</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6116666666666699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5366666666666702</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.46166666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3866666666666698</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2.31</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>2.2400000000000002</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>2.16</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>2.0870000000000002</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>2.0059999999999998</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>1.9279999999999999</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>1.849</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>1.7689999999999999</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>1.6910000000000001</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
                   <c:v>1.613</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
                   <c:v>1.5369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4587454545454499</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.38080909090909</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.3028727272727201</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2249363636363599</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -326,8 +407,8 @@
         <c:axId val="584351344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5"/>
-          <c:min val="-5"/>
+          <c:max val="10"/>
+          <c:min val="-10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -522,11 +603,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1526,13 +1607,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58CDC0C3-CC42-435D-94B9-9B790F9A24E3}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
   </cols>
@@ -1546,94 +1627,132 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2.6866666666666701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2.6116666666666699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2.5366666666666702</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2.46166666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2.3866666666666698</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B7" s="3">
         <v>2.31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B8" s="3">
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B9" s="3">
         <v>2.16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B10" s="3">
         <v>2.0870000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B11" s="3">
         <v>2.0059999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>0</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B12" s="3">
         <v>1.9279999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>-1</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B13" s="3">
         <v>1.849</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>-2</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B14" s="3">
         <v>1.7689999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>-3</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B15" s="3">
         <v>1.6910000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>-4</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B16" s="3">
         <v>1.613</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>-5</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B17" s="3">
         <v>1.5369999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>5</v>
       </c>
@@ -1641,12 +1760,56 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>-6</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1.4587454545454499</v>
+      </c>
       <c r="D18" t="s">
         <v>4</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>-7</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1.38080909090909</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>-8</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1.3028727272727201</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>-9</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1.2249363636363599</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>-10</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1.147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>